<commit_message>
Added Create and Read tests to project
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacqui.Muller\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janrich\Documents\NWU\323\Proj4\CMPG-323-Project-4---34894845\Connected Office Web Application User Acceptance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAB8EEF-425E-42A8-A7F1-FF25847C778D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CDA893-077E-4E00-8C94-5E34DEE6979A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="-15" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -687,7 +687,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,10 +1161,10 @@
         <v>57</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>0</v>
@@ -1178,10 +1178,10 @@
         <v>58</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>0</v>
@@ -1195,10 +1195,10 @@
         <v>59</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>0</v>
@@ -1212,10 +1212,10 @@
         <v>60</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>0</v>
@@ -1229,10 +1229,10 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>0</v>
@@ -1246,10 +1246,10 @@
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>0</v>
@@ -1263,10 +1263,10 @@
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="b">
         <v>0</v>
@@ -1280,10 +1280,10 @@
         <v>64</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>0</v>
@@ -1297,10 +1297,10 @@
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>0</v>
@@ -1314,10 +1314,10 @@
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="b">
         <v>0</v>
@@ -1331,10 +1331,10 @@
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="b">
         <v>0</v>
@@ -1348,10 +1348,10 @@
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="b">
         <v>0</v>
@@ -1365,10 +1365,10 @@
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="b">
         <v>0</v>
@@ -1382,10 +1382,10 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="b">
         <v>0</v>
@@ -1399,10 +1399,10 @@
         <v>48</v>
       </c>
       <c r="B16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="b">
         <v>0</v>
@@ -1416,10 +1416,10 @@
         <v>49</v>
       </c>
       <c r="B17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2" t="b">
         <v>0</v>
@@ -1433,10 +1433,10 @@
         <v>50</v>
       </c>
       <c r="B18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="b">
         <v>0</v>
@@ -1450,10 +1450,10 @@
         <v>51</v>
       </c>
       <c r="B19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2" t="b">
         <v>0</v>
@@ -1467,10 +1467,10 @@
         <v>52</v>
       </c>
       <c r="B20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2" t="b">
         <v>0</v>
@@ -1484,10 +1484,10 @@
         <v>53</v>
       </c>
       <c r="B21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="b">
         <v>0</v>
@@ -1501,10 +1501,10 @@
         <v>54</v>
       </c>
       <c r="B22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="b">
         <v>0</v>
@@ -1518,10 +1518,10 @@
         <v>55</v>
       </c>
       <c r="B23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="b">
         <v>0</v>
@@ -1535,10 +1535,10 @@
         <v>56</v>
       </c>
       <c r="B24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Finished with Update and Delete tests
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janrich\Documents\NWU\323\Proj4\CMPG-323-Project-4---34894845\Connected Office Web Application User Acceptance Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacqui.Muller\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CDA893-077E-4E00-8C94-5E34DEE6979A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAB8EEF-425E-42A8-A7F1-FF25847C778D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="-15" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -687,7 +687,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,10 +1161,10 @@
         <v>57</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>0</v>
@@ -1178,10 +1178,10 @@
         <v>58</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>0</v>
@@ -1195,10 +1195,10 @@
         <v>59</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>0</v>
@@ -1212,10 +1212,10 @@
         <v>60</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>0</v>
@@ -1229,10 +1229,10 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>0</v>
@@ -1246,10 +1246,10 @@
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>0</v>
@@ -1263,10 +1263,10 @@
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="b">
         <v>0</v>
@@ -1280,10 +1280,10 @@
         <v>64</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>0</v>
@@ -1297,10 +1297,10 @@
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>0</v>
@@ -1314,10 +1314,10 @@
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="b">
         <v>0</v>
@@ -1331,10 +1331,10 @@
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="b">
         <v>0</v>
@@ -1348,10 +1348,10 @@
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="b">
         <v>0</v>
@@ -1365,10 +1365,10 @@
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="b">
         <v>0</v>
@@ -1382,10 +1382,10 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="b">
         <v>0</v>
@@ -1399,10 +1399,10 @@
         <v>48</v>
       </c>
       <c r="B16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="b">
         <v>0</v>
@@ -1416,10 +1416,10 @@
         <v>49</v>
       </c>
       <c r="B17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2" t="b">
         <v>0</v>
@@ -1433,10 +1433,10 @@
         <v>50</v>
       </c>
       <c r="B18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2" t="b">
         <v>0</v>
@@ -1450,10 +1450,10 @@
         <v>51</v>
       </c>
       <c r="B19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="b">
         <v>0</v>
@@ -1467,10 +1467,10 @@
         <v>52</v>
       </c>
       <c r="B20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="2" t="b">
         <v>0</v>
@@ -1484,10 +1484,10 @@
         <v>53</v>
       </c>
       <c r="B21" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2" t="b">
         <v>0</v>
@@ -1501,10 +1501,10 @@
         <v>54</v>
       </c>
       <c r="B22" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2" t="b">
         <v>0</v>
@@ -1518,10 +1518,10 @@
         <v>55</v>
       </c>
       <c r="B23" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="2" t="b">
         <v>0</v>
@@ -1535,10 +1535,10 @@
         <v>56</v>
       </c>
       <c r="B24" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Final working UiPath project
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janrich\Documents\NWU\323\Proj4\CMPG-323-Project-4---34894845\Connected Office Web Application User Acceptance Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacqui.Muller\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BB52EB-D545-4E25-9812-3E7369FA0E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAB8EEF-425E-42A8-A7F1-FF25847C778D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="2595" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -1391,7 +1391,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1425,7 +1425,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1442,7 +1442,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1459,7 +1459,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1476,7 +1476,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1510,7 +1510,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1527,7 +1527,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>